<commit_message>
Add time frame selector with historical data support
- Add time frame presets: This Week, Last Week, This Month, Last Month, Last 3/6 Months, This Year, All Time, Custom
- Generate historical.json with all raw data for client-side filtering
- Aggregate data dynamically based on selected time frame
- Compare periods (current vs previous of same length)
- Custom date range picker with data availability indicator

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/reports/latest.xlsx
+++ b/reports/latest.xlsx
@@ -1064,14 +1064,14 @@
     </row>
     <row r="4">
       <c r="A4" s="11" t="n">
-        <v>22104</v>
+        <v>44208</v>
       </c>
       <c r="B4" s="11" t="n">
-        <v>390</v>
+        <v>780</v>
       </c>
       <c r="C4" s="11" t="inlineStr">
         <is>
-          <t>$57.30</t>
+          <t>$114.60</t>
         </is>
       </c>
       <c r="D4" s="11" t="inlineStr">
@@ -1083,7 +1083,7 @@
         <v>111</v>
       </c>
       <c r="F4" s="11" t="n">
-        <v>19</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6">
@@ -1156,23 +1156,23 @@
     <row r="9">
       <c r="A9" s="13" t="inlineStr">
         <is>
-          <t>Stop using V0 and Lovable to prototype, use Claude</t>
+          <t>I Built My Entire Design System in 4 Hours With AI</t>
         </is>
       </c>
       <c r="B9" s="13" t="n">
-        <v>2885</v>
+        <v>9874</v>
       </c>
       <c r="C9" s="13" t="n">
-        <v>40</v>
+        <v>227</v>
       </c>
       <c r="D9" s="13" t="inlineStr">
         <is>
-          <t>5.5%</t>
+          <t>6.8%</t>
         </is>
       </c>
       <c r="E9" s="13" t="inlineStr">
         <is>
-          <t>$11.36</t>
+          <t>$23.75</t>
         </is>
       </c>
       <c r="F9" s="13" t="inlineStr">
@@ -1184,23 +1184,23 @@
     <row r="10">
       <c r="A10" s="12" t="inlineStr">
         <is>
-          <t>How I Build a Component Library in 2 days (Figma t</t>
+          <t>Stop using V0 and Lovable to prototype, use Claude</t>
         </is>
       </c>
       <c r="B10" s="12" t="n">
-        <v>2352</v>
+        <v>2885</v>
       </c>
       <c r="C10" s="12" t="n">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="D10" s="12" t="inlineStr">
         <is>
-          <t>5.3%</t>
+          <t>5.5%</t>
         </is>
       </c>
       <c r="E10" s="12" t="inlineStr">
         <is>
-          <t>$12.74</t>
+          <t>$11.36</t>
         </is>
       </c>
       <c r="F10" s="12" t="inlineStr">
@@ -1212,23 +1212,23 @@
     <row r="11">
       <c r="A11" s="13" t="inlineStr">
         <is>
-          <t>Stop Wasting Dev Time on Frontend: Figma to Code i</t>
+          <t>Stop using V0 and Lovable to prototype, use Claude</t>
         </is>
       </c>
       <c r="B11" s="13" t="n">
-        <v>1247</v>
+        <v>2885</v>
       </c>
       <c r="C11" s="13" t="n">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="D11" s="13" t="inlineStr">
         <is>
-          <t>11.4%</t>
+          <t>5.5%</t>
         </is>
       </c>
       <c r="E11" s="13" t="inlineStr">
         <is>
-          <t>$1.76</t>
+          <t>$11.36</t>
         </is>
       </c>
       <c r="F11" s="13" t="inlineStr">
@@ -1240,23 +1240,23 @@
     <row r="12">
       <c r="A12" s="12" t="inlineStr">
         <is>
-          <t>Claude Code + Cursor + GitHub: The New AI environm</t>
+          <t>How I Build a Component Library in 2 days (Figma t</t>
         </is>
       </c>
       <c r="B12" s="12" t="n">
-        <v>999</v>
+        <v>2352</v>
       </c>
       <c r="C12" s="12" t="n">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="D12" s="12" t="inlineStr">
         <is>
-          <t>8.1%</t>
+          <t>5.3%</t>
         </is>
       </c>
       <c r="E12" s="12" t="inlineStr">
         <is>
-          <t>$4.72</t>
+          <t>$12.74</t>
         </is>
       </c>
       <c r="F12" s="12" t="inlineStr">
@@ -1268,51 +1268,51 @@
     <row r="13">
       <c r="A13" s="13" t="inlineStr">
         <is>
-          <t>Stop using V0 and Lovable to prototype, use Claude</t>
+          <t>How I Build a Component Library in 2 days (Figma t</t>
         </is>
       </c>
       <c r="B13" s="13" t="n">
-        <v>744</v>
+        <v>2352</v>
       </c>
       <c r="C13" s="13" t="n">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="D13" s="13" t="inlineStr">
         <is>
-          <t>0.4%</t>
+          <t>5.3%</t>
         </is>
       </c>
       <c r="E13" s="13" t="inlineStr">
         <is>
-          <t>$0.03</t>
+          <t>$12.74</t>
         </is>
       </c>
       <c r="F13" s="13" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="12" t="inlineStr">
         <is>
-          <t>Stop using V0 and Lovable to prototype, use Claude</t>
+          <t>Stop Wasting Dev Time on Frontend: Figma to Code i</t>
         </is>
       </c>
       <c r="B14" s="12" t="n">
-        <v>742</v>
+        <v>1247</v>
       </c>
       <c r="C14" s="12" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D14" s="12" t="inlineStr">
         <is>
-          <t>1.8%</t>
+          <t>11.4%</t>
         </is>
       </c>
       <c r="E14" s="12" t="inlineStr">
         <is>
-          <t>$0.03</t>
+          <t>$1.76</t>
         </is>
       </c>
       <c r="F14" s="12" t="inlineStr">
@@ -1324,23 +1324,23 @@
     <row r="15">
       <c r="A15" s="13" t="inlineStr">
         <is>
-          <t>Stop using V0 and Lovable to prototype, use Claude</t>
+          <t>Stop Wasting Dev Time on Frontend: Figma to Code i</t>
         </is>
       </c>
       <c r="B15" s="13" t="n">
-        <v>608</v>
+        <v>1247</v>
       </c>
       <c r="C15" s="13" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D15" s="13" t="inlineStr">
         <is>
-          <t>2.5%</t>
+          <t>11.4%</t>
         </is>
       </c>
       <c r="E15" s="13" t="inlineStr">
         <is>
-          <t>$0.03</t>
+          <t>$1.76</t>
         </is>
       </c>
       <c r="F15" s="13" t="inlineStr">
@@ -1352,23 +1352,23 @@
     <row r="16">
       <c r="A16" s="12" t="inlineStr">
         <is>
-          <t>Stop using V0 and Lovable to prototype, use Claude</t>
+          <t>Claude Code + Cursor + GitHub: The New AI environm</t>
         </is>
       </c>
       <c r="B16" s="12" t="n">
-        <v>449</v>
+        <v>999</v>
       </c>
       <c r="C16" s="12" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D16" s="12" t="inlineStr">
         <is>
-          <t>1.1%</t>
+          <t>8.1%</t>
         </is>
       </c>
       <c r="E16" s="12" t="inlineStr">
         <is>
-          <t>$0.01</t>
+          <t>$4.72</t>
         </is>
       </c>
       <c r="F16" s="12" t="inlineStr">
@@ -1380,23 +1380,23 @@
     <row r="17">
       <c r="A17" s="13" t="inlineStr">
         <is>
-          <t>I Tested Gemini 3 Pro vs Claude Opus 4.5 for UI De</t>
+          <t>Claude Code + Cursor + GitHub: The New AI environm</t>
         </is>
       </c>
       <c r="B17" s="13" t="n">
-        <v>411</v>
+        <v>999</v>
       </c>
       <c r="C17" s="13" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D17" s="13" t="inlineStr">
         <is>
-          <t>5.0%</t>
+          <t>8.1%</t>
         </is>
       </c>
       <c r="E17" s="13" t="inlineStr">
         <is>
-          <t>$0.92</t>
+          <t>$4.72</t>
         </is>
       </c>
       <c r="F17" s="13" t="inlineStr">

</xml_diff>